<commit_message>
Moving of tables greatly improved
</commit_message>
<xml_diff>
--- a/rations.xlsx
+++ b/rations.xlsx
@@ -409,7 +409,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:HF3019"/>
+  <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,56 +529,271 @@
     <row r="4" ht="13.5" customHeight="1" s="11">
       <c r="A4" s="7" t="n"/>
       <c r="E4" s="7" t="n"/>
-      <c r="Q4" s="7" t="n"/>
-      <c r="R4" s="7" t="n"/>
+      <c r="K4" s="7" t="inlineStr">
+        <is>
+          <t>Ration Table. List rations here with values for each ingredient in correct column, add ingredients to match ingredients table to end of table.</t>
+        </is>
+      </c>
+      <c r="L4" s="8" t="n"/>
+      <c r="M4" s="8" t="n"/>
+      <c r="N4" s="8" t="n"/>
+      <c r="O4" s="8" t="n"/>
+      <c r="P4" s="8" t="n"/>
+      <c r="Q4" s="8" t="n"/>
+      <c r="R4" s="8" t="n"/>
+      <c r="S4" s="8" t="n"/>
       <c r="T4" s="7" t="n"/>
-      <c r="W4" s="7" t="n"/>
-      <c r="X4" s="7" t="n"/>
-      <c r="Y4" s="7" t="n"/>
+      <c r="U4" s="8" t="n"/>
+      <c r="W4" s="7" t="inlineStr">
+        <is>
+          <t>House Table. List the house names here</t>
+        </is>
+      </c>
+      <c r="Y4" s="7" t="inlineStr">
+        <is>
+          <t>Weigher Table, gives weigher numbers and the value they increment by each time</t>
+        </is>
+      </c>
       <c r="Z4" s="7" t="n"/>
     </row>
     <row r="5" ht="13.5" customHeight="1" s="11">
       <c r="A5" s="7" t="n"/>
       <c r="E5" s="7" t="n"/>
-      <c r="Q5" s="7" t="n"/>
-      <c r="R5" s="7" t="n"/>
-      <c r="T5" s="7" t="n"/>
-      <c r="W5" s="7" t="n"/>
-      <c r="X5" s="7" t="n"/>
-      <c r="Y5" s="7" t="n"/>
-      <c r="Z5" s="7" t="n"/>
+      <c r="K5" s="4" t="inlineStr">
+        <is>
+          <t>Ration</t>
+        </is>
+      </c>
+      <c r="L5" s="5" t="inlineStr">
+        <is>
+          <t>Barley</t>
+        </is>
+      </c>
+      <c r="M5" s="5" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="N5" s="5" t="inlineStr">
+        <is>
+          <t>Soya</t>
+        </is>
+      </c>
+      <c r="O5" s="5" t="inlineStr">
+        <is>
+          <t>Limestone</t>
+        </is>
+      </c>
+      <c r="P5" s="5" t="inlineStr">
+        <is>
+          <t>Soya Oil</t>
+        </is>
+      </c>
+      <c r="Q5" s="5" t="inlineStr">
+        <is>
+          <t>Methionine</t>
+        </is>
+      </c>
+      <c r="R5" s="5" t="inlineStr">
+        <is>
+          <t>Arbocell</t>
+        </is>
+      </c>
+      <c r="S5" s="6" t="inlineStr">
+        <is>
+          <t>Premix</t>
+        </is>
+      </c>
+      <c r="T5" s="7" t="inlineStr">
+        <is>
+          <t>Extra Ingred</t>
+        </is>
+      </c>
+      <c r="U5" s="8" t="inlineStr">
+        <is>
+          <t>Extra Ingred 2</t>
+        </is>
+      </c>
+      <c r="W5" s="9" t="inlineStr">
+        <is>
+          <t>Houses</t>
+        </is>
+      </c>
+      <c r="Y5" s="7" t="inlineStr">
+        <is>
+          <t>Weighers</t>
+        </is>
+      </c>
+      <c r="Z5" s="7" t="inlineStr">
+        <is>
+          <t>Increment</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="13.5" customHeight="1" s="11">
       <c r="A6" s="7" t="n"/>
       <c r="E6" s="7" t="n"/>
-      <c r="Q6" s="7" t="n"/>
-      <c r="R6" s="7" t="n"/>
-      <c r="T6" s="7" t="n"/>
-      <c r="W6" s="7" t="n"/>
-      <c r="X6" s="7" t="n"/>
-      <c r="Y6" s="7" t="n"/>
-      <c r="Z6" s="7" t="n"/>
+      <c r="K6" s="7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" s="7" t="n">
+        <v>420</v>
+      </c>
+      <c r="U6" s="8" t="n"/>
+      <c r="W6" s="7" t="inlineStr">
+        <is>
+          <t>House 1</t>
+        </is>
+      </c>
+      <c r="Y6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="7" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" ht="13.5" customHeight="1" s="11">
       <c r="A7" s="7" t="n"/>
       <c r="E7" s="7" t="n"/>
-      <c r="Q7" s="7" t="n"/>
-      <c r="R7" s="7" t="n"/>
-      <c r="T7" s="7" t="n"/>
-      <c r="W7" s="7" t="n"/>
-      <c r="X7" s="7" t="n"/>
-      <c r="Y7" s="7" t="n"/>
-      <c r="Z7" s="7" t="n"/>
+      <c r="G7" s="7" t="inlineStr">
+        <is>
+          <t>Ingredients Table. List ingredients here with their respective weigher number and relative ordering (ordering is individual to each weigher, leave both blank if they are manually added).</t>
+        </is>
+      </c>
+      <c r="H7" s="8" t="n"/>
+      <c r="I7" s="8" t="n"/>
+      <c r="K7" s="7" t="inlineStr">
+        <is>
+          <t>Peak Lay</t>
+        </is>
+      </c>
+      <c r="L7" s="7" t="n">
+        <v>300</v>
+      </c>
+      <c r="M7" s="7" t="n">
+        <v>560</v>
+      </c>
+      <c r="N7" s="7" t="n">
+        <v>210</v>
+      </c>
+      <c r="O7" s="7" t="n">
+        <v>58</v>
+      </c>
+      <c r="P7" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q7" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="R7" s="7" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="S7" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="T7" s="7" t="n">
+        <v>32</v>
+      </c>
+      <c r="U7" s="8" t="n">
+        <v>32</v>
+      </c>
+      <c r="W7" s="7" t="inlineStr">
+        <is>
+          <t>House 2</t>
+        </is>
+      </c>
+      <c r="Y7" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z7" s="7" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" ht="13.5" customHeight="1" s="11">
       <c r="A8" s="7" t="n"/>
       <c r="E8" s="7" t="n"/>
-      <c r="Q8" s="7" t="n"/>
-      <c r="R8" s="7" t="n"/>
-      <c r="T8" s="7" t="n"/>
-      <c r="U8" s="7" t="n"/>
+      <c r="G8" s="4" t="inlineStr">
+        <is>
+          <t>Ingredient</t>
+        </is>
+      </c>
+      <c r="H8" s="5" t="inlineStr">
+        <is>
+          <t>Weigher</t>
+        </is>
+      </c>
+      <c r="I8" s="6" t="inlineStr">
+        <is>
+          <t>Ordering</t>
+        </is>
+      </c>
+      <c r="K8" s="7" t="inlineStr">
+        <is>
+          <t>Mid Lay</t>
+        </is>
+      </c>
+      <c r="L8" s="7" t="n">
+        <v>50</v>
+      </c>
+      <c r="M8" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="N8" s="7" t="n">
+        <v>62</v>
+      </c>
+      <c r="O8" s="7" t="n">
+        <v>51</v>
+      </c>
+      <c r="P8" s="7" t="n">
+        <v>866</v>
+      </c>
+      <c r="Q8" s="7" t="n">
+        <v>23</v>
+      </c>
+      <c r="R8" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="S8" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="T8" s="7" t="n">
+        <v>32</v>
+      </c>
+      <c r="U8" s="8" t="n">
+        <v>32</v>
+      </c>
       <c r="V8" s="7" t="n"/>
-      <c r="W8" s="7" t="n"/>
+      <c r="W8" s="7" t="inlineStr">
+        <is>
+          <t>House 3</t>
+        </is>
+      </c>
       <c r="X8" s="7" t="n"/>
       <c r="Y8" s="7" t="n"/>
       <c r="Z8" s="7" t="n"/>
@@ -586,12 +801,56 @@
     <row r="9" ht="13.5" customHeight="1" s="11">
       <c r="A9" s="7" t="n"/>
       <c r="E9" s="7" t="n"/>
-      <c r="Q9" s="7" t="n"/>
-      <c r="R9" s="7" t="n"/>
-      <c r="T9" s="7" t="n"/>
-      <c r="U9" s="7" t="n"/>
+      <c r="G9" s="7" t="inlineStr">
+        <is>
+          <t>Barley</t>
+        </is>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" s="7" t="inlineStr">
+        <is>
+          <t>Other Ration 1</t>
+        </is>
+      </c>
+      <c r="L9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="7" t="n"/>
+      <c r="O9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" s="7" t="n">
+        <v>32</v>
+      </c>
+      <c r="U9" s="8" t="n">
+        <v>32</v>
+      </c>
       <c r="V9" s="7" t="n"/>
-      <c r="W9" s="7" t="n"/>
+      <c r="W9" s="7" t="inlineStr">
+        <is>
+          <t>Manor Wood</t>
+        </is>
+      </c>
       <c r="X9" s="7" t="n"/>
       <c r="Y9" s="7" t="n"/>
       <c r="Z9" s="7" t="n"/>
@@ -599,12 +858,58 @@
     <row r="10" ht="13.5" customHeight="1" s="11">
       <c r="A10" s="7" t="n"/>
       <c r="E10" s="7" t="n"/>
-      <c r="Q10" s="7" t="n"/>
-      <c r="R10" s="7" t="n"/>
-      <c r="T10" s="7" t="n"/>
-      <c r="U10" s="7" t="n"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="H10" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="K10" s="7" t="inlineStr">
+        <is>
+          <t>Other Ration 2</t>
+        </is>
+      </c>
+      <c r="L10" s="7" t="n">
+        <v>300</v>
+      </c>
+      <c r="M10" s="7" t="n">
+        <v>560</v>
+      </c>
+      <c r="N10" s="7" t="n">
+        <v>210</v>
+      </c>
+      <c r="O10" s="7" t="n">
+        <v>58</v>
+      </c>
+      <c r="P10" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q10" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="R10" s="7" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="S10" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="T10" s="7" t="n">
+        <v>32</v>
+      </c>
+      <c r="U10" s="8" t="n">
+        <v>32</v>
+      </c>
       <c r="V10" s="7" t="n"/>
-      <c r="W10" s="7" t="n"/>
+      <c r="W10" s="7" t="inlineStr">
+        <is>
+          <t>Wawne Hill</t>
+        </is>
+      </c>
       <c r="X10" s="7" t="n"/>
       <c r="Y10" s="7" t="n"/>
       <c r="Z10" s="7" t="n"/>
@@ -612,12 +917,56 @@
     <row r="11" ht="13.5" customHeight="1" s="11">
       <c r="A11" s="7" t="n"/>
       <c r="E11" s="7" t="n"/>
-      <c r="Q11" s="7" t="n"/>
-      <c r="R11" s="7" t="n"/>
-      <c r="T11" s="7" t="n"/>
+      <c r="G11" s="7" t="inlineStr">
+        <is>
+          <t>Soya</t>
+        </is>
+      </c>
+      <c r="H11" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="7" t="inlineStr">
+        <is>
+          <t>Other Ration 3</t>
+        </is>
+      </c>
+      <c r="L11" s="7" t="n">
+        <v>50</v>
+      </c>
+      <c r="M11" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="N11" s="7" t="n">
+        <v>62</v>
+      </c>
+      <c r="O11" s="7" t="n">
+        <v>51</v>
+      </c>
+      <c r="P11" s="7" t="n">
+        <v>866</v>
+      </c>
+      <c r="Q11" s="7" t="n">
+        <v>23</v>
+      </c>
+      <c r="R11" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="S11" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="T11" s="7" t="n">
+        <v>32</v>
+      </c>
       <c r="U11" s="7" t="n"/>
       <c r="V11" s="7" t="n"/>
-      <c r="W11" s="7" t="n"/>
+      <c r="W11" s="7" t="inlineStr">
+        <is>
+          <t>House 4</t>
+        </is>
+      </c>
       <c r="X11" s="7" t="n"/>
       <c r="Y11" s="7" t="n"/>
       <c r="Z11" s="7" t="n"/>
@@ -625,12 +974,56 @@
     <row r="12" ht="13.5" customHeight="1" s="11">
       <c r="A12" s="7" t="n"/>
       <c r="E12" s="7" t="n"/>
-      <c r="Q12" s="7" t="n"/>
-      <c r="R12" s="7" t="n"/>
-      <c r="T12" s="7" t="n"/>
+      <c r="G12" s="7" t="inlineStr">
+        <is>
+          <t>Limestone</t>
+        </is>
+      </c>
+      <c r="H12" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K12" s="7" t="inlineStr">
+        <is>
+          <t>Other Ration 4</t>
+        </is>
+      </c>
+      <c r="L12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" s="7" t="n">
+        <v>32</v>
+      </c>
       <c r="U12" s="7" t="n"/>
       <c r="V12" s="7" t="n"/>
-      <c r="W12" s="7" t="n"/>
+      <c r="W12" s="7" t="inlineStr">
+        <is>
+          <t>House 5</t>
+        </is>
+      </c>
       <c r="X12" s="7" t="n"/>
       <c r="Y12" s="7" t="n"/>
       <c r="Z12" s="7" t="n"/>
@@ -638,12 +1031,56 @@
     <row r="13" ht="13.5" customHeight="1" s="11">
       <c r="A13" s="7" t="n"/>
       <c r="E13" s="7" t="n"/>
-      <c r="Q13" s="7" t="n"/>
-      <c r="R13" s="7" t="n"/>
-      <c r="T13" s="7" t="n"/>
+      <c r="G13" s="10" t="inlineStr">
+        <is>
+          <t>Extra Ingred</t>
+        </is>
+      </c>
+      <c r="H13" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="K13" s="7" t="inlineStr">
+        <is>
+          <t>Other Ration 5</t>
+        </is>
+      </c>
+      <c r="L13" s="7" t="n">
+        <v>300</v>
+      </c>
+      <c r="M13" s="7" t="n">
+        <v>560</v>
+      </c>
+      <c r="N13" s="7" t="n">
+        <v>210</v>
+      </c>
+      <c r="O13" s="7" t="n">
+        <v>58</v>
+      </c>
+      <c r="P13" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q13" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="R13" s="7" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="S13" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="T13" s="7" t="n">
+        <v>32</v>
+      </c>
       <c r="U13" s="7" t="n"/>
       <c r="V13" s="7" t="n"/>
-      <c r="W13" s="7" t="n"/>
+      <c r="W13" s="7" t="inlineStr">
+        <is>
+          <t>House 6</t>
+        </is>
+      </c>
       <c r="X13" s="7" t="n"/>
       <c r="Y13" s="7" t="n"/>
       <c r="Z13" s="7" t="n"/>
@@ -651,12 +1088,56 @@
     <row r="14" ht="13.5" customHeight="1" s="11">
       <c r="A14" s="7" t="n"/>
       <c r="E14" s="7" t="n"/>
-      <c r="Q14" s="7" t="n"/>
-      <c r="R14" s="7" t="n"/>
-      <c r="T14" s="7" t="n"/>
+      <c r="G14" s="10" t="inlineStr">
+        <is>
+          <t>Extra Ingred 2</t>
+        </is>
+      </c>
+      <c r="H14" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="I14" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="7" t="inlineStr">
+        <is>
+          <t>Other Ration 6</t>
+        </is>
+      </c>
+      <c r="L14" s="7" t="n">
+        <v>50</v>
+      </c>
+      <c r="M14" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="N14" s="7" t="n">
+        <v>62</v>
+      </c>
+      <c r="O14" s="7" t="n">
+        <v>51</v>
+      </c>
+      <c r="P14" s="7" t="n">
+        <v>866</v>
+      </c>
+      <c r="Q14" s="7" t="n">
+        <v>23</v>
+      </c>
+      <c r="R14" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="S14" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="T14" s="7" t="n">
+        <v>32</v>
+      </c>
       <c r="U14" s="7" t="n"/>
       <c r="V14" s="7" t="n"/>
-      <c r="W14" s="7" t="n"/>
+      <c r="W14" s="7" t="inlineStr">
+        <is>
+          <t>House 7</t>
+        </is>
+      </c>
       <c r="X14" s="7" t="n"/>
       <c r="Y14" s="7" t="n"/>
       <c r="Z14" s="7" t="n"/>
@@ -664,12 +1145,50 @@
     <row r="15" ht="13.5" customHeight="1" s="11">
       <c r="A15" s="7" t="n"/>
       <c r="E15" s="7" t="n"/>
-      <c r="Q15" s="7" t="n"/>
-      <c r="R15" s="7" t="n"/>
-      <c r="T15" s="7" t="n"/>
+      <c r="G15" s="7" t="inlineStr">
+        <is>
+          <t>Soya Oil</t>
+        </is>
+      </c>
+      <c r="H15" s="7" t="n"/>
+      <c r="I15" s="7" t="n"/>
+      <c r="K15" s="7" t="inlineStr">
+        <is>
+          <t>Other Ration 7</t>
+        </is>
+      </c>
+      <c r="L15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" s="7" t="n"/>
+      <c r="P15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" s="7" t="n">
+        <v>600</v>
+      </c>
       <c r="U15" s="7" t="n"/>
       <c r="V15" s="7" t="n"/>
-      <c r="W15" s="7" t="n"/>
+      <c r="W15" s="7" t="inlineStr">
+        <is>
+          <t>House 8</t>
+        </is>
+      </c>
       <c r="X15" s="7" t="n"/>
       <c r="Y15" s="7" t="n"/>
       <c r="Z15" s="7" t="n"/>
@@ -680,12 +1199,50 @@
       <c r="C16" s="7" t="n"/>
       <c r="D16" s="7" t="n"/>
       <c r="E16" s="7" t="n"/>
-      <c r="Q16" s="7" t="n"/>
-      <c r="R16" s="7" t="n"/>
+      <c r="G16" s="7" t="inlineStr">
+        <is>
+          <t>Methionine</t>
+        </is>
+      </c>
+      <c r="H16" s="7" t="n"/>
+      <c r="I16" s="7" t="n"/>
+      <c r="K16" s="7" t="inlineStr">
+        <is>
+          <t>Other Ration 8</t>
+        </is>
+      </c>
+      <c r="L16" s="7" t="n">
+        <v>300</v>
+      </c>
+      <c r="M16" s="7" t="n">
+        <v>560</v>
+      </c>
+      <c r="N16" s="7" t="n">
+        <v>210</v>
+      </c>
+      <c r="O16" s="7" t="n">
+        <v>58</v>
+      </c>
+      <c r="P16" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q16" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="R16" s="7" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="S16" s="7" t="n">
+        <v>40</v>
+      </c>
       <c r="T16" s="7" t="n"/>
       <c r="U16" s="7" t="n"/>
       <c r="V16" s="7" t="n"/>
-      <c r="W16" s="7" t="n"/>
+      <c r="W16" s="7" t="inlineStr">
+        <is>
+          <t>House 9</t>
+        </is>
+      </c>
       <c r="X16" s="7" t="n"/>
       <c r="Y16" s="7" t="n"/>
       <c r="Z16" s="7" t="n"/>
@@ -696,12 +1253,50 @@
       <c r="C17" s="7" t="n"/>
       <c r="D17" s="7" t="n"/>
       <c r="E17" s="7" t="n"/>
-      <c r="Q17" s="7" t="n"/>
-      <c r="R17" s="7" t="n"/>
+      <c r="G17" s="7" t="inlineStr">
+        <is>
+          <t>Arbocell</t>
+        </is>
+      </c>
+      <c r="H17" s="7" t="n"/>
+      <c r="I17" s="7" t="n"/>
+      <c r="K17" s="7" t="inlineStr">
+        <is>
+          <t>Other Ration 9</t>
+        </is>
+      </c>
+      <c r="L17" s="7" t="n">
+        <v>50</v>
+      </c>
+      <c r="M17" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="N17" s="7" t="n">
+        <v>62</v>
+      </c>
+      <c r="O17" s="7" t="n">
+        <v>51</v>
+      </c>
+      <c r="P17" s="7" t="n">
+        <v>866</v>
+      </c>
+      <c r="Q17" s="7" t="n">
+        <v>23</v>
+      </c>
+      <c r="R17" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="S17" s="7" t="n">
+        <v>4</v>
+      </c>
       <c r="T17" s="7" t="n"/>
       <c r="U17" s="7" t="n"/>
       <c r="V17" s="7" t="n"/>
-      <c r="W17" s="7" t="n"/>
+      <c r="W17" s="7" t="inlineStr">
+        <is>
+          <t>House 10</t>
+        </is>
+      </c>
       <c r="X17" s="7" t="n"/>
       <c r="Y17" s="7" t="n"/>
       <c r="Z17" s="7" t="n"/>
@@ -713,7 +1308,11 @@
       <c r="D18" s="7" t="n"/>
       <c r="E18" s="7" t="n"/>
       <c r="F18" s="7" t="n"/>
-      <c r="G18" s="7" t="n"/>
+      <c r="G18" s="7" t="inlineStr">
+        <is>
+          <t>Premix</t>
+        </is>
+      </c>
       <c r="H18" s="7" t="n"/>
       <c r="I18" s="7" t="n"/>
       <c r="J18" s="7" t="n"/>
@@ -728,7 +1327,11 @@
       <c r="T18" s="7" t="n"/>
       <c r="U18" s="7" t="n"/>
       <c r="V18" s="7" t="n"/>
-      <c r="W18" s="7" t="n"/>
+      <c r="W18" s="7" t="inlineStr">
+        <is>
+          <t>House 11</t>
+        </is>
+      </c>
       <c r="X18" s="7" t="n"/>
       <c r="Y18" s="7" t="n"/>
       <c r="Z18" s="7" t="n"/>
@@ -755,7 +1358,11 @@
       <c r="T19" s="7" t="n"/>
       <c r="U19" s="7" t="n"/>
       <c r="V19" s="7" t="n"/>
-      <c r="W19" s="7" t="n"/>
+      <c r="W19" s="7" t="inlineStr">
+        <is>
+          <t>House 12</t>
+        </is>
+      </c>
       <c r="X19" s="7" t="n"/>
       <c r="Y19" s="7" t="n"/>
       <c r="Z19" s="7" t="n"/>
@@ -7168,2731 +7775,6 @@
     <row r="998" ht="15.75" customHeight="1" s="11"/>
     <row r="999" ht="15.75" customHeight="1" s="11"/>
     <row r="1000" ht="15.75" customHeight="1" s="11"/>
-    <row r="1001"/>
-    <row r="1002"/>
-    <row r="1003"/>
-    <row r="1004"/>
-    <row r="1005"/>
-    <row r="1006"/>
-    <row r="1007"/>
-    <row r="1008"/>
-    <row r="1009"/>
-    <row r="1010"/>
-    <row r="1011"/>
-    <row r="1012"/>
-    <row r="1013"/>
-    <row r="1014"/>
-    <row r="1015"/>
-    <row r="1016"/>
-    <row r="1017"/>
-    <row r="1018"/>
-    <row r="1019"/>
-    <row r="1020"/>
-    <row r="1021"/>
-    <row r="1022"/>
-    <row r="1023"/>
-    <row r="1024"/>
-    <row r="1025"/>
-    <row r="1026"/>
-    <row r="1027"/>
-    <row r="1028"/>
-    <row r="1029"/>
-    <row r="1030"/>
-    <row r="1031"/>
-    <row r="1032"/>
-    <row r="1033"/>
-    <row r="1034"/>
-    <row r="1035"/>
-    <row r="1036"/>
-    <row r="1037"/>
-    <row r="1038"/>
-    <row r="1039"/>
-    <row r="1040"/>
-    <row r="1041"/>
-    <row r="1042"/>
-    <row r="1043"/>
-    <row r="1044"/>
-    <row r="1045"/>
-    <row r="1046"/>
-    <row r="1047"/>
-    <row r="1048"/>
-    <row r="1049"/>
-    <row r="1050"/>
-    <row r="1051"/>
-    <row r="1052"/>
-    <row r="1053"/>
-    <row r="1054"/>
-    <row r="1055"/>
-    <row r="1056"/>
-    <row r="1057"/>
-    <row r="1058"/>
-    <row r="1059"/>
-    <row r="1060"/>
-    <row r="1061"/>
-    <row r="1062"/>
-    <row r="1063"/>
-    <row r="1064"/>
-    <row r="1065"/>
-    <row r="1066"/>
-    <row r="1067"/>
-    <row r="1068"/>
-    <row r="1069"/>
-    <row r="1070"/>
-    <row r="1071"/>
-    <row r="1072"/>
-    <row r="1073"/>
-    <row r="1074"/>
-    <row r="1075"/>
-    <row r="1076"/>
-    <row r="1077"/>
-    <row r="1078"/>
-    <row r="1079"/>
-    <row r="1080"/>
-    <row r="1081"/>
-    <row r="1082"/>
-    <row r="1083"/>
-    <row r="1084"/>
-    <row r="1085"/>
-    <row r="1086"/>
-    <row r="1087"/>
-    <row r="1088"/>
-    <row r="1089"/>
-    <row r="1090"/>
-    <row r="1091"/>
-    <row r="1092"/>
-    <row r="1093"/>
-    <row r="1094"/>
-    <row r="1095"/>
-    <row r="1096"/>
-    <row r="1097"/>
-    <row r="1098"/>
-    <row r="1099"/>
-    <row r="1100"/>
-    <row r="1101"/>
-    <row r="1102"/>
-    <row r="1103"/>
-    <row r="1104"/>
-    <row r="1105"/>
-    <row r="1106"/>
-    <row r="1107"/>
-    <row r="1108"/>
-    <row r="1109"/>
-    <row r="1110"/>
-    <row r="1111"/>
-    <row r="1112"/>
-    <row r="1113"/>
-    <row r="1114"/>
-    <row r="1115"/>
-    <row r="1116"/>
-    <row r="1117"/>
-    <row r="1118"/>
-    <row r="1119"/>
-    <row r="1120"/>
-    <row r="1121"/>
-    <row r="1122"/>
-    <row r="1123"/>
-    <row r="1124"/>
-    <row r="1125"/>
-    <row r="1126"/>
-    <row r="1127"/>
-    <row r="1128"/>
-    <row r="1129"/>
-    <row r="1130"/>
-    <row r="1131"/>
-    <row r="1132"/>
-    <row r="1133"/>
-    <row r="1134"/>
-    <row r="1135"/>
-    <row r="1136"/>
-    <row r="1137"/>
-    <row r="1138"/>
-    <row r="1139"/>
-    <row r="1140"/>
-    <row r="1141"/>
-    <row r="1142"/>
-    <row r="1143"/>
-    <row r="1144"/>
-    <row r="1145"/>
-    <row r="1146"/>
-    <row r="1147"/>
-    <row r="1148"/>
-    <row r="1149"/>
-    <row r="1150"/>
-    <row r="1151"/>
-    <row r="1152"/>
-    <row r="1153"/>
-    <row r="1154"/>
-    <row r="1155"/>
-    <row r="1156"/>
-    <row r="1157"/>
-    <row r="1158"/>
-    <row r="1159"/>
-    <row r="1160"/>
-    <row r="1161"/>
-    <row r="1162"/>
-    <row r="1163"/>
-    <row r="1164"/>
-    <row r="1165"/>
-    <row r="1166"/>
-    <row r="1167"/>
-    <row r="1168"/>
-    <row r="1169"/>
-    <row r="1170"/>
-    <row r="1171"/>
-    <row r="1172"/>
-    <row r="1173"/>
-    <row r="1174"/>
-    <row r="1175"/>
-    <row r="1176"/>
-    <row r="1177"/>
-    <row r="1178"/>
-    <row r="1179"/>
-    <row r="1180"/>
-    <row r="1181"/>
-    <row r="1182"/>
-    <row r="1183"/>
-    <row r="1184"/>
-    <row r="1185"/>
-    <row r="1186"/>
-    <row r="1187"/>
-    <row r="1188"/>
-    <row r="1189"/>
-    <row r="1190"/>
-    <row r="1191"/>
-    <row r="1192"/>
-    <row r="1193"/>
-    <row r="1194"/>
-    <row r="1195"/>
-    <row r="1196"/>
-    <row r="1197"/>
-    <row r="1198"/>
-    <row r="1199"/>
-    <row r="1200"/>
-    <row r="1201"/>
-    <row r="1202"/>
-    <row r="1203"/>
-    <row r="1204"/>
-    <row r="1205"/>
-    <row r="1206"/>
-    <row r="1207"/>
-    <row r="1208"/>
-    <row r="1209"/>
-    <row r="1210"/>
-    <row r="1211"/>
-    <row r="1212"/>
-    <row r="1213"/>
-    <row r="1214"/>
-    <row r="1215"/>
-    <row r="1216"/>
-    <row r="1217"/>
-    <row r="1218"/>
-    <row r="1219"/>
-    <row r="1220"/>
-    <row r="1221"/>
-    <row r="1222"/>
-    <row r="1223"/>
-    <row r="1224"/>
-    <row r="1225"/>
-    <row r="1226"/>
-    <row r="1227"/>
-    <row r="1228"/>
-    <row r="1229"/>
-    <row r="1230"/>
-    <row r="1231"/>
-    <row r="1232"/>
-    <row r="1233"/>
-    <row r="1234"/>
-    <row r="1235"/>
-    <row r="1236"/>
-    <row r="1237"/>
-    <row r="1238"/>
-    <row r="1239"/>
-    <row r="1240"/>
-    <row r="1241"/>
-    <row r="1242"/>
-    <row r="1243"/>
-    <row r="1244"/>
-    <row r="1245"/>
-    <row r="1246"/>
-    <row r="1247"/>
-    <row r="1248"/>
-    <row r="1249"/>
-    <row r="1250"/>
-    <row r="1251"/>
-    <row r="1252"/>
-    <row r="1253"/>
-    <row r="1254"/>
-    <row r="1255"/>
-    <row r="1256"/>
-    <row r="1257"/>
-    <row r="1258"/>
-    <row r="1259"/>
-    <row r="1260"/>
-    <row r="1261"/>
-    <row r="1262"/>
-    <row r="1263"/>
-    <row r="1264"/>
-    <row r="1265"/>
-    <row r="1266"/>
-    <row r="1267"/>
-    <row r="1268"/>
-    <row r="1269"/>
-    <row r="1270"/>
-    <row r="1271"/>
-    <row r="1272"/>
-    <row r="1273"/>
-    <row r="1274"/>
-    <row r="1275"/>
-    <row r="1276"/>
-    <row r="1277"/>
-    <row r="1278"/>
-    <row r="1279"/>
-    <row r="1280"/>
-    <row r="1281"/>
-    <row r="1282"/>
-    <row r="1283"/>
-    <row r="1284"/>
-    <row r="1285"/>
-    <row r="1286"/>
-    <row r="1287"/>
-    <row r="1288"/>
-    <row r="1289"/>
-    <row r="1290"/>
-    <row r="1291"/>
-    <row r="1292"/>
-    <row r="1293"/>
-    <row r="1294"/>
-    <row r="1295"/>
-    <row r="1296"/>
-    <row r="1297"/>
-    <row r="1298"/>
-    <row r="1299"/>
-    <row r="1300"/>
-    <row r="1301"/>
-    <row r="1302"/>
-    <row r="1303"/>
-    <row r="1304"/>
-    <row r="1305"/>
-    <row r="1306"/>
-    <row r="1307"/>
-    <row r="1308"/>
-    <row r="1309"/>
-    <row r="1310"/>
-    <row r="1311"/>
-    <row r="1312"/>
-    <row r="1313"/>
-    <row r="1314"/>
-    <row r="1315"/>
-    <row r="1316"/>
-    <row r="1317"/>
-    <row r="1318"/>
-    <row r="1319"/>
-    <row r="1320"/>
-    <row r="1321"/>
-    <row r="1322"/>
-    <row r="1323"/>
-    <row r="1324"/>
-    <row r="1325"/>
-    <row r="1326"/>
-    <row r="1327"/>
-    <row r="1328"/>
-    <row r="1329"/>
-    <row r="1330"/>
-    <row r="1331"/>
-    <row r="1332"/>
-    <row r="1333"/>
-    <row r="1334"/>
-    <row r="1335"/>
-    <row r="1336"/>
-    <row r="1337"/>
-    <row r="1338"/>
-    <row r="1339"/>
-    <row r="1340"/>
-    <row r="1341"/>
-    <row r="1342"/>
-    <row r="1343"/>
-    <row r="1344"/>
-    <row r="1345"/>
-    <row r="1346"/>
-    <row r="1347"/>
-    <row r="1348"/>
-    <row r="1349"/>
-    <row r="1350"/>
-    <row r="1351"/>
-    <row r="1352"/>
-    <row r="1353"/>
-    <row r="1354"/>
-    <row r="1355"/>
-    <row r="1356"/>
-    <row r="1357"/>
-    <row r="1358"/>
-    <row r="1359"/>
-    <row r="1360"/>
-    <row r="1361"/>
-    <row r="1362"/>
-    <row r="1363"/>
-    <row r="1364"/>
-    <row r="1365"/>
-    <row r="1366"/>
-    <row r="1367"/>
-    <row r="1368"/>
-    <row r="1369"/>
-    <row r="1370"/>
-    <row r="1371"/>
-    <row r="1372"/>
-    <row r="1373"/>
-    <row r="1374"/>
-    <row r="1375"/>
-    <row r="1376"/>
-    <row r="1377"/>
-    <row r="1378"/>
-    <row r="1379"/>
-    <row r="1380"/>
-    <row r="1381"/>
-    <row r="1382"/>
-    <row r="1383"/>
-    <row r="1384"/>
-    <row r="1385"/>
-    <row r="1386"/>
-    <row r="1387"/>
-    <row r="1388"/>
-    <row r="1389"/>
-    <row r="1390"/>
-    <row r="1391"/>
-    <row r="1392"/>
-    <row r="1393"/>
-    <row r="1394"/>
-    <row r="1395"/>
-    <row r="1396"/>
-    <row r="1397"/>
-    <row r="1398"/>
-    <row r="1399"/>
-    <row r="1400"/>
-    <row r="1401"/>
-    <row r="1402"/>
-    <row r="1403"/>
-    <row r="1404"/>
-    <row r="1405"/>
-    <row r="1406"/>
-    <row r="1407"/>
-    <row r="1408"/>
-    <row r="1409"/>
-    <row r="1410"/>
-    <row r="1411"/>
-    <row r="1412"/>
-    <row r="1413"/>
-    <row r="1414"/>
-    <row r="1415"/>
-    <row r="1416"/>
-    <row r="1417"/>
-    <row r="1418"/>
-    <row r="1419"/>
-    <row r="1420"/>
-    <row r="1421"/>
-    <row r="1422"/>
-    <row r="1423"/>
-    <row r="1424"/>
-    <row r="1425"/>
-    <row r="1426"/>
-    <row r="1427"/>
-    <row r="1428"/>
-    <row r="1429"/>
-    <row r="1430"/>
-    <row r="1431"/>
-    <row r="1432"/>
-    <row r="1433"/>
-    <row r="1434"/>
-    <row r="1435"/>
-    <row r="1436"/>
-    <row r="1437"/>
-    <row r="1438"/>
-    <row r="1439"/>
-    <row r="1440"/>
-    <row r="1441"/>
-    <row r="1442"/>
-    <row r="1443"/>
-    <row r="1444"/>
-    <row r="1445"/>
-    <row r="1446"/>
-    <row r="1447"/>
-    <row r="1448"/>
-    <row r="1449"/>
-    <row r="1450"/>
-    <row r="1451"/>
-    <row r="1452"/>
-    <row r="1453"/>
-    <row r="1454"/>
-    <row r="1455"/>
-    <row r="1456"/>
-    <row r="1457"/>
-    <row r="1458"/>
-    <row r="1459"/>
-    <row r="1460"/>
-    <row r="1461"/>
-    <row r="1462"/>
-    <row r="1463"/>
-    <row r="1464"/>
-    <row r="1465"/>
-    <row r="1466"/>
-    <row r="1467"/>
-    <row r="1468"/>
-    <row r="1469"/>
-    <row r="1470"/>
-    <row r="1471"/>
-    <row r="1472"/>
-    <row r="1473"/>
-    <row r="1474"/>
-    <row r="1475"/>
-    <row r="1476"/>
-    <row r="1477"/>
-    <row r="1478"/>
-    <row r="1479"/>
-    <row r="1480"/>
-    <row r="1481"/>
-    <row r="1482"/>
-    <row r="1483"/>
-    <row r="1484"/>
-    <row r="1485"/>
-    <row r="1486"/>
-    <row r="1487"/>
-    <row r="1488"/>
-    <row r="1489"/>
-    <row r="1490"/>
-    <row r="1491"/>
-    <row r="1492"/>
-    <row r="1493"/>
-    <row r="1494"/>
-    <row r="1495"/>
-    <row r="1496"/>
-    <row r="1497"/>
-    <row r="1498"/>
-    <row r="1499"/>
-    <row r="1500"/>
-    <row r="1501"/>
-    <row r="1502"/>
-    <row r="1503"/>
-    <row r="1504"/>
-    <row r="1505"/>
-    <row r="1506"/>
-    <row r="1507"/>
-    <row r="1508"/>
-    <row r="1509"/>
-    <row r="1510"/>
-    <row r="1511"/>
-    <row r="1512"/>
-    <row r="1513"/>
-    <row r="1514"/>
-    <row r="1515"/>
-    <row r="1516"/>
-    <row r="1517"/>
-    <row r="1518"/>
-    <row r="1519"/>
-    <row r="1520"/>
-    <row r="1521"/>
-    <row r="1522"/>
-    <row r="1523"/>
-    <row r="1524"/>
-    <row r="1525"/>
-    <row r="1526"/>
-    <row r="1527"/>
-    <row r="1528"/>
-    <row r="1529"/>
-    <row r="1530"/>
-    <row r="1531"/>
-    <row r="1532"/>
-    <row r="1533"/>
-    <row r="1534"/>
-    <row r="1535"/>
-    <row r="1536"/>
-    <row r="1537"/>
-    <row r="1538"/>
-    <row r="1539"/>
-    <row r="1540"/>
-    <row r="1541"/>
-    <row r="1542"/>
-    <row r="1543"/>
-    <row r="1544"/>
-    <row r="1545"/>
-    <row r="1546"/>
-    <row r="1547"/>
-    <row r="1548"/>
-    <row r="1549"/>
-    <row r="1550"/>
-    <row r="1551"/>
-    <row r="1552"/>
-    <row r="1553"/>
-    <row r="1554"/>
-    <row r="1555"/>
-    <row r="1556"/>
-    <row r="1557"/>
-    <row r="1558"/>
-    <row r="1559"/>
-    <row r="1560"/>
-    <row r="1561"/>
-    <row r="1562"/>
-    <row r="1563"/>
-    <row r="1564"/>
-    <row r="1565"/>
-    <row r="1566"/>
-    <row r="1567"/>
-    <row r="1568"/>
-    <row r="1569"/>
-    <row r="1570"/>
-    <row r="1571"/>
-    <row r="1572"/>
-    <row r="1573"/>
-    <row r="1574"/>
-    <row r="1575"/>
-    <row r="1576"/>
-    <row r="1577"/>
-    <row r="1578"/>
-    <row r="1579"/>
-    <row r="1580"/>
-    <row r="1581"/>
-    <row r="1582"/>
-    <row r="1583"/>
-    <row r="1584"/>
-    <row r="1585"/>
-    <row r="1586"/>
-    <row r="1587"/>
-    <row r="1588"/>
-    <row r="1589"/>
-    <row r="1590"/>
-    <row r="1591"/>
-    <row r="1592"/>
-    <row r="1593"/>
-    <row r="1594"/>
-    <row r="1595"/>
-    <row r="1596"/>
-    <row r="1597"/>
-    <row r="1598"/>
-    <row r="1599"/>
-    <row r="1600"/>
-    <row r="1601"/>
-    <row r="1602"/>
-    <row r="1603"/>
-    <row r="1604"/>
-    <row r="1605"/>
-    <row r="1606"/>
-    <row r="1607"/>
-    <row r="1608"/>
-    <row r="1609"/>
-    <row r="1610"/>
-    <row r="1611"/>
-    <row r="1612"/>
-    <row r="1613"/>
-    <row r="1614"/>
-    <row r="1615"/>
-    <row r="1616"/>
-    <row r="1617"/>
-    <row r="1618"/>
-    <row r="1619"/>
-    <row r="1620"/>
-    <row r="1621"/>
-    <row r="1622"/>
-    <row r="1623"/>
-    <row r="1624"/>
-    <row r="1625"/>
-    <row r="1626"/>
-    <row r="1627"/>
-    <row r="1628"/>
-    <row r="1629"/>
-    <row r="1630"/>
-    <row r="1631"/>
-    <row r="1632"/>
-    <row r="1633"/>
-    <row r="1634"/>
-    <row r="1635"/>
-    <row r="1636"/>
-    <row r="1637"/>
-    <row r="1638"/>
-    <row r="1639"/>
-    <row r="1640"/>
-    <row r="1641"/>
-    <row r="1642"/>
-    <row r="1643"/>
-    <row r="1644"/>
-    <row r="1645"/>
-    <row r="1646"/>
-    <row r="1647"/>
-    <row r="1648"/>
-    <row r="1649"/>
-    <row r="1650"/>
-    <row r="1651"/>
-    <row r="1652"/>
-    <row r="1653"/>
-    <row r="1654"/>
-    <row r="1655"/>
-    <row r="1656"/>
-    <row r="1657"/>
-    <row r="1658"/>
-    <row r="1659"/>
-    <row r="1660"/>
-    <row r="1661"/>
-    <row r="1662"/>
-    <row r="1663"/>
-    <row r="1664"/>
-    <row r="1665"/>
-    <row r="1666"/>
-    <row r="1667"/>
-    <row r="1668"/>
-    <row r="1669"/>
-    <row r="1670"/>
-    <row r="1671"/>
-    <row r="1672"/>
-    <row r="1673"/>
-    <row r="1674"/>
-    <row r="1675"/>
-    <row r="1676"/>
-    <row r="1677"/>
-    <row r="1678"/>
-    <row r="1679"/>
-    <row r="1680"/>
-    <row r="1681"/>
-    <row r="1682"/>
-    <row r="1683"/>
-    <row r="1684"/>
-    <row r="1685"/>
-    <row r="1686"/>
-    <row r="1687"/>
-    <row r="1688"/>
-    <row r="1689"/>
-    <row r="1690"/>
-    <row r="1691"/>
-    <row r="1692"/>
-    <row r="1693"/>
-    <row r="1694"/>
-    <row r="1695"/>
-    <row r="1696"/>
-    <row r="1697"/>
-    <row r="1698"/>
-    <row r="1699"/>
-    <row r="1700"/>
-    <row r="1701"/>
-    <row r="1702"/>
-    <row r="1703"/>
-    <row r="1704"/>
-    <row r="1705"/>
-    <row r="1706"/>
-    <row r="1707"/>
-    <row r="1708"/>
-    <row r="1709"/>
-    <row r="1710"/>
-    <row r="1711"/>
-    <row r="1712"/>
-    <row r="1713"/>
-    <row r="1714"/>
-    <row r="1715"/>
-    <row r="1716"/>
-    <row r="1717"/>
-    <row r="1718"/>
-    <row r="1719"/>
-    <row r="1720"/>
-    <row r="1721"/>
-    <row r="1722"/>
-    <row r="1723"/>
-    <row r="1724"/>
-    <row r="1725"/>
-    <row r="1726"/>
-    <row r="1727"/>
-    <row r="1728"/>
-    <row r="1729"/>
-    <row r="1730"/>
-    <row r="1731"/>
-    <row r="1732"/>
-    <row r="1733"/>
-    <row r="1734"/>
-    <row r="1735"/>
-    <row r="1736"/>
-    <row r="1737"/>
-    <row r="1738"/>
-    <row r="1739"/>
-    <row r="1740"/>
-    <row r="1741"/>
-    <row r="1742"/>
-    <row r="1743"/>
-    <row r="1744"/>
-    <row r="1745"/>
-    <row r="1746"/>
-    <row r="1747"/>
-    <row r="1748"/>
-    <row r="1749"/>
-    <row r="1750"/>
-    <row r="1751"/>
-    <row r="1752"/>
-    <row r="1753"/>
-    <row r="1754"/>
-    <row r="1755"/>
-    <row r="1756"/>
-    <row r="1757"/>
-    <row r="1758"/>
-    <row r="1759"/>
-    <row r="1760"/>
-    <row r="1761"/>
-    <row r="1762"/>
-    <row r="1763"/>
-    <row r="1764"/>
-    <row r="1765"/>
-    <row r="1766"/>
-    <row r="1767"/>
-    <row r="1768"/>
-    <row r="1769"/>
-    <row r="1770"/>
-    <row r="1771"/>
-    <row r="1772"/>
-    <row r="1773"/>
-    <row r="1774"/>
-    <row r="1775"/>
-    <row r="1776"/>
-    <row r="1777"/>
-    <row r="1778"/>
-    <row r="1779"/>
-    <row r="1780"/>
-    <row r="1781"/>
-    <row r="1782"/>
-    <row r="1783"/>
-    <row r="1784"/>
-    <row r="1785"/>
-    <row r="1786"/>
-    <row r="1787"/>
-    <row r="1788"/>
-    <row r="1789"/>
-    <row r="1790"/>
-    <row r="1791"/>
-    <row r="1792"/>
-    <row r="1793"/>
-    <row r="1794"/>
-    <row r="1795"/>
-    <row r="1796"/>
-    <row r="1797"/>
-    <row r="1798"/>
-    <row r="1799"/>
-    <row r="1800"/>
-    <row r="1801"/>
-    <row r="1802"/>
-    <row r="1803"/>
-    <row r="1804"/>
-    <row r="1805"/>
-    <row r="1806"/>
-    <row r="1807"/>
-    <row r="1808"/>
-    <row r="1809"/>
-    <row r="1810"/>
-    <row r="1811"/>
-    <row r="1812"/>
-    <row r="1813"/>
-    <row r="1814"/>
-    <row r="1815"/>
-    <row r="1816"/>
-    <row r="1817"/>
-    <row r="1818"/>
-    <row r="1819"/>
-    <row r="1820"/>
-    <row r="1821"/>
-    <row r="1822"/>
-    <row r="1823"/>
-    <row r="1824"/>
-    <row r="1825"/>
-    <row r="1826"/>
-    <row r="1827"/>
-    <row r="1828"/>
-    <row r="1829"/>
-    <row r="1830"/>
-    <row r="1831"/>
-    <row r="1832"/>
-    <row r="1833"/>
-    <row r="1834"/>
-    <row r="1835"/>
-    <row r="1836"/>
-    <row r="1837"/>
-    <row r="1838"/>
-    <row r="1839"/>
-    <row r="1840"/>
-    <row r="1841"/>
-    <row r="1842"/>
-    <row r="1843"/>
-    <row r="1844"/>
-    <row r="1845"/>
-    <row r="1846"/>
-    <row r="1847"/>
-    <row r="1848"/>
-    <row r="1849"/>
-    <row r="1850"/>
-    <row r="1851"/>
-    <row r="1852"/>
-    <row r="1853"/>
-    <row r="1854"/>
-    <row r="1855"/>
-    <row r="1856"/>
-    <row r="1857"/>
-    <row r="1858"/>
-    <row r="1859"/>
-    <row r="1860"/>
-    <row r="1861"/>
-    <row r="1862"/>
-    <row r="1863"/>
-    <row r="1864"/>
-    <row r="1865"/>
-    <row r="1866"/>
-    <row r="1867"/>
-    <row r="1868"/>
-    <row r="1869"/>
-    <row r="1870"/>
-    <row r="1871"/>
-    <row r="1872"/>
-    <row r="1873"/>
-    <row r="1874"/>
-    <row r="1875"/>
-    <row r="1876"/>
-    <row r="1877"/>
-    <row r="1878"/>
-    <row r="1879"/>
-    <row r="1880"/>
-    <row r="1881"/>
-    <row r="1882"/>
-    <row r="1883"/>
-    <row r="1884"/>
-    <row r="1885"/>
-    <row r="1886"/>
-    <row r="1887"/>
-    <row r="1888"/>
-    <row r="1889"/>
-    <row r="1890"/>
-    <row r="1891"/>
-    <row r="1892"/>
-    <row r="1893"/>
-    <row r="1894"/>
-    <row r="1895"/>
-    <row r="1896"/>
-    <row r="1897"/>
-    <row r="1898"/>
-    <row r="1899"/>
-    <row r="1900"/>
-    <row r="1901"/>
-    <row r="1902"/>
-    <row r="1903"/>
-    <row r="1904"/>
-    <row r="1905"/>
-    <row r="1906"/>
-    <row r="1907"/>
-    <row r="1908"/>
-    <row r="1909"/>
-    <row r="1910"/>
-    <row r="1911"/>
-    <row r="1912"/>
-    <row r="1913"/>
-    <row r="1914"/>
-    <row r="1915"/>
-    <row r="1916"/>
-    <row r="1917"/>
-    <row r="1918"/>
-    <row r="1919"/>
-    <row r="1920"/>
-    <row r="1921"/>
-    <row r="1922"/>
-    <row r="1923"/>
-    <row r="1924"/>
-    <row r="1925"/>
-    <row r="1926"/>
-    <row r="1927"/>
-    <row r="1928"/>
-    <row r="1929"/>
-    <row r="1930"/>
-    <row r="1931"/>
-    <row r="1932"/>
-    <row r="1933"/>
-    <row r="1934"/>
-    <row r="1935"/>
-    <row r="1936"/>
-    <row r="1937"/>
-    <row r="1938"/>
-    <row r="1939"/>
-    <row r="1940"/>
-    <row r="1941"/>
-    <row r="1942"/>
-    <row r="1943"/>
-    <row r="1944"/>
-    <row r="1945"/>
-    <row r="1946"/>
-    <row r="1947"/>
-    <row r="1948"/>
-    <row r="1949"/>
-    <row r="1950"/>
-    <row r="1951"/>
-    <row r="1952"/>
-    <row r="1953"/>
-    <row r="1954"/>
-    <row r="1955"/>
-    <row r="1956"/>
-    <row r="1957"/>
-    <row r="1958"/>
-    <row r="1959"/>
-    <row r="1960"/>
-    <row r="1961"/>
-    <row r="1962"/>
-    <row r="1963"/>
-    <row r="1964"/>
-    <row r="1965"/>
-    <row r="1966"/>
-    <row r="1967"/>
-    <row r="1968"/>
-    <row r="1969"/>
-    <row r="1970"/>
-    <row r="1971"/>
-    <row r="1972"/>
-    <row r="1973"/>
-    <row r="1974"/>
-    <row r="1975"/>
-    <row r="1976"/>
-    <row r="1977"/>
-    <row r="1978"/>
-    <row r="1979"/>
-    <row r="1980"/>
-    <row r="1981"/>
-    <row r="1982"/>
-    <row r="1983"/>
-    <row r="1984"/>
-    <row r="1985"/>
-    <row r="1986"/>
-    <row r="1987"/>
-    <row r="1988"/>
-    <row r="1989"/>
-    <row r="1990"/>
-    <row r="1991"/>
-    <row r="1992"/>
-    <row r="1993"/>
-    <row r="1994"/>
-    <row r="1995"/>
-    <row r="1996"/>
-    <row r="1997"/>
-    <row r="1998"/>
-    <row r="1999"/>
-    <row r="2000"/>
-    <row r="2001"/>
-    <row r="2002"/>
-    <row r="2003"/>
-    <row r="2004"/>
-    <row r="2005"/>
-    <row r="2006"/>
-    <row r="2007"/>
-    <row r="2008"/>
-    <row r="2009"/>
-    <row r="2010"/>
-    <row r="2011"/>
-    <row r="2012"/>
-    <row r="2013"/>
-    <row r="2014"/>
-    <row r="2015"/>
-    <row r="2016"/>
-    <row r="2017"/>
-    <row r="2018"/>
-    <row r="2019"/>
-    <row r="2020"/>
-    <row r="2021"/>
-    <row r="2022"/>
-    <row r="2023"/>
-    <row r="2024"/>
-    <row r="2025"/>
-    <row r="2026"/>
-    <row r="2027"/>
-    <row r="2028"/>
-    <row r="2029"/>
-    <row r="2030"/>
-    <row r="2031"/>
-    <row r="2032"/>
-    <row r="2033"/>
-    <row r="2034"/>
-    <row r="2035"/>
-    <row r="2036"/>
-    <row r="2037"/>
-    <row r="2038"/>
-    <row r="2039"/>
-    <row r="2040"/>
-    <row r="2041"/>
-    <row r="2042"/>
-    <row r="2043"/>
-    <row r="2044"/>
-    <row r="2045"/>
-    <row r="2046"/>
-    <row r="2047"/>
-    <row r="2048"/>
-    <row r="2049"/>
-    <row r="2050"/>
-    <row r="2051"/>
-    <row r="2052"/>
-    <row r="2053"/>
-    <row r="2054"/>
-    <row r="2055"/>
-    <row r="2056"/>
-    <row r="2057"/>
-    <row r="2058"/>
-    <row r="2059"/>
-    <row r="2060"/>
-    <row r="2061"/>
-    <row r="2062"/>
-    <row r="2063"/>
-    <row r="2064"/>
-    <row r="2065"/>
-    <row r="2066"/>
-    <row r="2067"/>
-    <row r="2068"/>
-    <row r="2069"/>
-    <row r="2070"/>
-    <row r="2071"/>
-    <row r="2072"/>
-    <row r="2073"/>
-    <row r="2074"/>
-    <row r="2075"/>
-    <row r="2076"/>
-    <row r="2077"/>
-    <row r="2078"/>
-    <row r="2079"/>
-    <row r="2080"/>
-    <row r="2081"/>
-    <row r="2082"/>
-    <row r="2083"/>
-    <row r="2084"/>
-    <row r="2085"/>
-    <row r="2086"/>
-    <row r="2087"/>
-    <row r="2088"/>
-    <row r="2089"/>
-    <row r="2090"/>
-    <row r="2091"/>
-    <row r="2092"/>
-    <row r="2093"/>
-    <row r="2094"/>
-    <row r="2095"/>
-    <row r="2096"/>
-    <row r="2097"/>
-    <row r="2098"/>
-    <row r="2099"/>
-    <row r="2100"/>
-    <row r="2101"/>
-    <row r="2102"/>
-    <row r="2103"/>
-    <row r="2104"/>
-    <row r="2105"/>
-    <row r="2106"/>
-    <row r="2107"/>
-    <row r="2108"/>
-    <row r="2109"/>
-    <row r="2110"/>
-    <row r="2111"/>
-    <row r="2112"/>
-    <row r="2113"/>
-    <row r="2114"/>
-    <row r="2115"/>
-    <row r="2116"/>
-    <row r="2117"/>
-    <row r="2118"/>
-    <row r="2119"/>
-    <row r="2120"/>
-    <row r="2121"/>
-    <row r="2122"/>
-    <row r="2123"/>
-    <row r="2124"/>
-    <row r="2125"/>
-    <row r="2126"/>
-    <row r="2127"/>
-    <row r="2128"/>
-    <row r="2129"/>
-    <row r="2130"/>
-    <row r="2131"/>
-    <row r="2132"/>
-    <row r="2133"/>
-    <row r="2134"/>
-    <row r="2135"/>
-    <row r="2136"/>
-    <row r="2137"/>
-    <row r="2138"/>
-    <row r="2139"/>
-    <row r="2140"/>
-    <row r="2141"/>
-    <row r="2142"/>
-    <row r="2143"/>
-    <row r="2144"/>
-    <row r="2145"/>
-    <row r="2146"/>
-    <row r="2147"/>
-    <row r="2148"/>
-    <row r="2149"/>
-    <row r="2150"/>
-    <row r="2151"/>
-    <row r="2152"/>
-    <row r="2153"/>
-    <row r="2154"/>
-    <row r="2155"/>
-    <row r="2156"/>
-    <row r="2157"/>
-    <row r="2158"/>
-    <row r="2159"/>
-    <row r="2160"/>
-    <row r="2161"/>
-    <row r="2162"/>
-    <row r="2163"/>
-    <row r="2164"/>
-    <row r="2165"/>
-    <row r="2166"/>
-    <row r="2167"/>
-    <row r="2168"/>
-    <row r="2169"/>
-    <row r="2170"/>
-    <row r="2171"/>
-    <row r="2172"/>
-    <row r="2173"/>
-    <row r="2174"/>
-    <row r="2175"/>
-    <row r="2176"/>
-    <row r="2177"/>
-    <row r="2178"/>
-    <row r="2179"/>
-    <row r="2180"/>
-    <row r="2181"/>
-    <row r="2182"/>
-    <row r="2183"/>
-    <row r="2184"/>
-    <row r="2185"/>
-    <row r="2186"/>
-    <row r="2187"/>
-    <row r="2188"/>
-    <row r="2189"/>
-    <row r="2190"/>
-    <row r="2191"/>
-    <row r="2192"/>
-    <row r="2193"/>
-    <row r="2194"/>
-    <row r="2195"/>
-    <row r="2196"/>
-    <row r="2197"/>
-    <row r="2198"/>
-    <row r="2199"/>
-    <row r="2200"/>
-    <row r="2201"/>
-    <row r="2202"/>
-    <row r="2203"/>
-    <row r="2204"/>
-    <row r="2205"/>
-    <row r="2206"/>
-    <row r="2207"/>
-    <row r="2208"/>
-    <row r="2209"/>
-    <row r="2210"/>
-    <row r="2211"/>
-    <row r="2212"/>
-    <row r="2213"/>
-    <row r="2214"/>
-    <row r="2215"/>
-    <row r="2216"/>
-    <row r="2217"/>
-    <row r="2218"/>
-    <row r="2219"/>
-    <row r="2220"/>
-    <row r="2221"/>
-    <row r="2222"/>
-    <row r="2223"/>
-    <row r="2224"/>
-    <row r="2225"/>
-    <row r="2226"/>
-    <row r="2227"/>
-    <row r="2228"/>
-    <row r="2229"/>
-    <row r="2230"/>
-    <row r="2231"/>
-    <row r="2232"/>
-    <row r="2233"/>
-    <row r="2234"/>
-    <row r="2235"/>
-    <row r="2236"/>
-    <row r="2237"/>
-    <row r="2238"/>
-    <row r="2239"/>
-    <row r="2240"/>
-    <row r="2241"/>
-    <row r="2242"/>
-    <row r="2243"/>
-    <row r="2244"/>
-    <row r="2245"/>
-    <row r="2246"/>
-    <row r="2247"/>
-    <row r="2248"/>
-    <row r="2249"/>
-    <row r="2250"/>
-    <row r="2251"/>
-    <row r="2252"/>
-    <row r="2253"/>
-    <row r="2254"/>
-    <row r="2255"/>
-    <row r="2256"/>
-    <row r="2257"/>
-    <row r="2258"/>
-    <row r="2259"/>
-    <row r="2260"/>
-    <row r="2261"/>
-    <row r="2262"/>
-    <row r="2263"/>
-    <row r="2264"/>
-    <row r="2265"/>
-    <row r="2266"/>
-    <row r="2267"/>
-    <row r="2268"/>
-    <row r="2269"/>
-    <row r="2270"/>
-    <row r="2271"/>
-    <row r="2272"/>
-    <row r="2273"/>
-    <row r="2274"/>
-    <row r="2275"/>
-    <row r="2276"/>
-    <row r="2277"/>
-    <row r="2278"/>
-    <row r="2279"/>
-    <row r="2280"/>
-    <row r="2281"/>
-    <row r="2282"/>
-    <row r="2283"/>
-    <row r="2284"/>
-    <row r="2285"/>
-    <row r="2286"/>
-    <row r="2287"/>
-    <row r="2288"/>
-    <row r="2289"/>
-    <row r="2290"/>
-    <row r="2291"/>
-    <row r="2292"/>
-    <row r="2293"/>
-    <row r="2294"/>
-    <row r="2295"/>
-    <row r="2296"/>
-    <row r="2297"/>
-    <row r="2298"/>
-    <row r="2299"/>
-    <row r="2300"/>
-    <row r="2301"/>
-    <row r="2302"/>
-    <row r="2303"/>
-    <row r="2304"/>
-    <row r="2305"/>
-    <row r="2306"/>
-    <row r="2307"/>
-    <row r="2308"/>
-    <row r="2309"/>
-    <row r="2310"/>
-    <row r="2311"/>
-    <row r="2312"/>
-    <row r="2313"/>
-    <row r="2314"/>
-    <row r="2315"/>
-    <row r="2316"/>
-    <row r="2317"/>
-    <row r="2318"/>
-    <row r="2319"/>
-    <row r="2320"/>
-    <row r="2321"/>
-    <row r="2322"/>
-    <row r="2323"/>
-    <row r="2324"/>
-    <row r="2325"/>
-    <row r="2326"/>
-    <row r="2327"/>
-    <row r="2328"/>
-    <row r="2329"/>
-    <row r="2330"/>
-    <row r="2331"/>
-    <row r="2332"/>
-    <row r="2333"/>
-    <row r="2334"/>
-    <row r="2335"/>
-    <row r="2336"/>
-    <row r="2337"/>
-    <row r="2338"/>
-    <row r="2339"/>
-    <row r="2340"/>
-    <row r="2341"/>
-    <row r="2342"/>
-    <row r="2343"/>
-    <row r="2344"/>
-    <row r="2345"/>
-    <row r="2346"/>
-    <row r="2347"/>
-    <row r="2348"/>
-    <row r="2349"/>
-    <row r="2350"/>
-    <row r="2351"/>
-    <row r="2352"/>
-    <row r="2353"/>
-    <row r="2354"/>
-    <row r="2355"/>
-    <row r="2356"/>
-    <row r="2357"/>
-    <row r="2358"/>
-    <row r="2359"/>
-    <row r="2360"/>
-    <row r="2361"/>
-    <row r="2362"/>
-    <row r="2363"/>
-    <row r="2364"/>
-    <row r="2365"/>
-    <row r="2366"/>
-    <row r="2367"/>
-    <row r="2368"/>
-    <row r="2369"/>
-    <row r="2370"/>
-    <row r="2371"/>
-    <row r="2372"/>
-    <row r="2373"/>
-    <row r="2374"/>
-    <row r="2375"/>
-    <row r="2376"/>
-    <row r="2377"/>
-    <row r="2378"/>
-    <row r="2379"/>
-    <row r="2380"/>
-    <row r="2381"/>
-    <row r="2382"/>
-    <row r="2383"/>
-    <row r="2384"/>
-    <row r="2385"/>
-    <row r="2386"/>
-    <row r="2387"/>
-    <row r="2388"/>
-    <row r="2389"/>
-    <row r="2390"/>
-    <row r="2391"/>
-    <row r="2392"/>
-    <row r="2393"/>
-    <row r="2394"/>
-    <row r="2395"/>
-    <row r="2396"/>
-    <row r="2397"/>
-    <row r="2398"/>
-    <row r="2399"/>
-    <row r="2400"/>
-    <row r="2401"/>
-    <row r="2402"/>
-    <row r="2403"/>
-    <row r="2404"/>
-    <row r="2405"/>
-    <row r="2406"/>
-    <row r="2407"/>
-    <row r="2408"/>
-    <row r="2409"/>
-    <row r="2410"/>
-    <row r="2411"/>
-    <row r="2412"/>
-    <row r="2413"/>
-    <row r="2414"/>
-    <row r="2415"/>
-    <row r="2416"/>
-    <row r="2417"/>
-    <row r="2418"/>
-    <row r="2419"/>
-    <row r="2420"/>
-    <row r="2421"/>
-    <row r="2422"/>
-    <row r="2423"/>
-    <row r="2424"/>
-    <row r="2425"/>
-    <row r="2426"/>
-    <row r="2427"/>
-    <row r="2428"/>
-    <row r="2429"/>
-    <row r="2430"/>
-    <row r="2431"/>
-    <row r="2432"/>
-    <row r="2433"/>
-    <row r="2434"/>
-    <row r="2435"/>
-    <row r="2436"/>
-    <row r="2437"/>
-    <row r="2438"/>
-    <row r="2439"/>
-    <row r="2440"/>
-    <row r="2441"/>
-    <row r="2442"/>
-    <row r="2443"/>
-    <row r="2444"/>
-    <row r="2445"/>
-    <row r="2446"/>
-    <row r="2447"/>
-    <row r="2448"/>
-    <row r="2449"/>
-    <row r="2450"/>
-    <row r="2451"/>
-    <row r="2452"/>
-    <row r="2453"/>
-    <row r="2454"/>
-    <row r="2455"/>
-    <row r="2456"/>
-    <row r="2457"/>
-    <row r="2458"/>
-    <row r="2459"/>
-    <row r="2460"/>
-    <row r="2461"/>
-    <row r="2462"/>
-    <row r="2463"/>
-    <row r="2464"/>
-    <row r="2465"/>
-    <row r="2466"/>
-    <row r="2467"/>
-    <row r="2468"/>
-    <row r="2469"/>
-    <row r="2470"/>
-    <row r="2471"/>
-    <row r="2472"/>
-    <row r="2473"/>
-    <row r="2474"/>
-    <row r="2475"/>
-    <row r="2476"/>
-    <row r="2477"/>
-    <row r="2478"/>
-    <row r="2479"/>
-    <row r="2480"/>
-    <row r="2481"/>
-    <row r="2482"/>
-    <row r="2483"/>
-    <row r="2484"/>
-    <row r="2485"/>
-    <row r="2486"/>
-    <row r="2487"/>
-    <row r="2488"/>
-    <row r="2489"/>
-    <row r="2490"/>
-    <row r="2491"/>
-    <row r="2492"/>
-    <row r="2493"/>
-    <row r="2494"/>
-    <row r="2495"/>
-    <row r="2496"/>
-    <row r="2497"/>
-    <row r="2498"/>
-    <row r="2499"/>
-    <row r="2500"/>
-    <row r="2501"/>
-    <row r="2502"/>
-    <row r="2503"/>
-    <row r="2504"/>
-    <row r="2505"/>
-    <row r="2506"/>
-    <row r="2507"/>
-    <row r="2508"/>
-    <row r="2509"/>
-    <row r="2510"/>
-    <row r="2511"/>
-    <row r="2512"/>
-    <row r="2513"/>
-    <row r="2514"/>
-    <row r="2515"/>
-    <row r="2516"/>
-    <row r="2517"/>
-    <row r="2518"/>
-    <row r="2519"/>
-    <row r="2520"/>
-    <row r="2521"/>
-    <row r="2522"/>
-    <row r="2523"/>
-    <row r="2524"/>
-    <row r="2525"/>
-    <row r="2526"/>
-    <row r="2527"/>
-    <row r="2528"/>
-    <row r="2529"/>
-    <row r="2530"/>
-    <row r="2531"/>
-    <row r="2532"/>
-    <row r="2533"/>
-    <row r="2534"/>
-    <row r="2535"/>
-    <row r="2536"/>
-    <row r="2537"/>
-    <row r="2538"/>
-    <row r="2539"/>
-    <row r="2540"/>
-    <row r="2541"/>
-    <row r="2542"/>
-    <row r="2543"/>
-    <row r="2544"/>
-    <row r="2545"/>
-    <row r="2546"/>
-    <row r="2547"/>
-    <row r="2548"/>
-    <row r="2549"/>
-    <row r="2550"/>
-    <row r="2551"/>
-    <row r="2552"/>
-    <row r="2553"/>
-    <row r="2554"/>
-    <row r="2555"/>
-    <row r="2556"/>
-    <row r="2557"/>
-    <row r="2558"/>
-    <row r="2559"/>
-    <row r="2560"/>
-    <row r="2561"/>
-    <row r="2562"/>
-    <row r="2563"/>
-    <row r="2564"/>
-    <row r="2565"/>
-    <row r="2566"/>
-    <row r="2567"/>
-    <row r="2568"/>
-    <row r="2569"/>
-    <row r="2570"/>
-    <row r="2571"/>
-    <row r="2572"/>
-    <row r="2573"/>
-    <row r="2574"/>
-    <row r="2575"/>
-    <row r="2576"/>
-    <row r="2577"/>
-    <row r="2578"/>
-    <row r="2579"/>
-    <row r="2580"/>
-    <row r="2581"/>
-    <row r="2582"/>
-    <row r="2583"/>
-    <row r="2584"/>
-    <row r="2585"/>
-    <row r="2586"/>
-    <row r="2587"/>
-    <row r="2588"/>
-    <row r="2589"/>
-    <row r="2590"/>
-    <row r="2591"/>
-    <row r="2592"/>
-    <row r="2593"/>
-    <row r="2594"/>
-    <row r="2595"/>
-    <row r="2596"/>
-    <row r="2597"/>
-    <row r="2598"/>
-    <row r="2599"/>
-    <row r="2600"/>
-    <row r="2601"/>
-    <row r="2602"/>
-    <row r="2603"/>
-    <row r="2604"/>
-    <row r="2605"/>
-    <row r="2606"/>
-    <row r="2607"/>
-    <row r="2608"/>
-    <row r="2609"/>
-    <row r="2610"/>
-    <row r="2611"/>
-    <row r="2612"/>
-    <row r="2613"/>
-    <row r="2614"/>
-    <row r="2615"/>
-    <row r="2616"/>
-    <row r="2617"/>
-    <row r="2618"/>
-    <row r="2619"/>
-    <row r="2620"/>
-    <row r="2621"/>
-    <row r="2622"/>
-    <row r="2623"/>
-    <row r="2624"/>
-    <row r="2625"/>
-    <row r="2626"/>
-    <row r="2627"/>
-    <row r="2628"/>
-    <row r="2629"/>
-    <row r="2630"/>
-    <row r="2631"/>
-    <row r="2632"/>
-    <row r="2633"/>
-    <row r="2634"/>
-    <row r="2635"/>
-    <row r="2636"/>
-    <row r="2637"/>
-    <row r="2638"/>
-    <row r="2639"/>
-    <row r="2640"/>
-    <row r="2641"/>
-    <row r="2642"/>
-    <row r="2643"/>
-    <row r="2644"/>
-    <row r="2645"/>
-    <row r="2646"/>
-    <row r="2647"/>
-    <row r="2648"/>
-    <row r="2649"/>
-    <row r="2650"/>
-    <row r="2651"/>
-    <row r="2652"/>
-    <row r="2653"/>
-    <row r="2654"/>
-    <row r="2655"/>
-    <row r="2656"/>
-    <row r="2657"/>
-    <row r="2658"/>
-    <row r="2659"/>
-    <row r="2660"/>
-    <row r="2661"/>
-    <row r="2662"/>
-    <row r="2663"/>
-    <row r="2664"/>
-    <row r="2665"/>
-    <row r="2666"/>
-    <row r="2667"/>
-    <row r="2668"/>
-    <row r="2669"/>
-    <row r="2670"/>
-    <row r="2671"/>
-    <row r="2672"/>
-    <row r="2673"/>
-    <row r="2674"/>
-    <row r="2675"/>
-    <row r="2676"/>
-    <row r="2677"/>
-    <row r="2678"/>
-    <row r="2679"/>
-    <row r="2680"/>
-    <row r="2681"/>
-    <row r="2682"/>
-    <row r="2683"/>
-    <row r="2684"/>
-    <row r="2685"/>
-    <row r="2686"/>
-    <row r="2687"/>
-    <row r="2688"/>
-    <row r="2689"/>
-    <row r="2690"/>
-    <row r="2691"/>
-    <row r="2692"/>
-    <row r="2693"/>
-    <row r="2694"/>
-    <row r="2695"/>
-    <row r="2696"/>
-    <row r="2697"/>
-    <row r="2698"/>
-    <row r="2699"/>
-    <row r="2700"/>
-    <row r="2701"/>
-    <row r="2702"/>
-    <row r="2703"/>
-    <row r="2704"/>
-    <row r="2705"/>
-    <row r="2706"/>
-    <row r="2707"/>
-    <row r="2708"/>
-    <row r="2709"/>
-    <row r="2710"/>
-    <row r="2711"/>
-    <row r="2712"/>
-    <row r="2713"/>
-    <row r="2714"/>
-    <row r="2715"/>
-    <row r="2716"/>
-    <row r="2717"/>
-    <row r="2718"/>
-    <row r="2719"/>
-    <row r="2720"/>
-    <row r="2721"/>
-    <row r="2722"/>
-    <row r="2723"/>
-    <row r="2724"/>
-    <row r="2725"/>
-    <row r="2726"/>
-    <row r="2727"/>
-    <row r="2728"/>
-    <row r="2729"/>
-    <row r="2730"/>
-    <row r="2731"/>
-    <row r="2732"/>
-    <row r="2733"/>
-    <row r="2734"/>
-    <row r="2735"/>
-    <row r="2736"/>
-    <row r="2737"/>
-    <row r="2738"/>
-    <row r="2739"/>
-    <row r="2740"/>
-    <row r="2741"/>
-    <row r="2742"/>
-    <row r="2743"/>
-    <row r="2744"/>
-    <row r="2745"/>
-    <row r="2746"/>
-    <row r="2747"/>
-    <row r="2748"/>
-    <row r="2749"/>
-    <row r="2750"/>
-    <row r="2751"/>
-    <row r="2752"/>
-    <row r="2753"/>
-    <row r="2754"/>
-    <row r="2755"/>
-    <row r="2756"/>
-    <row r="2757"/>
-    <row r="2758"/>
-    <row r="2759"/>
-    <row r="2760"/>
-    <row r="2761"/>
-    <row r="2762"/>
-    <row r="2763"/>
-    <row r="2764"/>
-    <row r="2765"/>
-    <row r="2766"/>
-    <row r="2767"/>
-    <row r="2768"/>
-    <row r="2769"/>
-    <row r="2770"/>
-    <row r="2771"/>
-    <row r="2772"/>
-    <row r="2773"/>
-    <row r="2774"/>
-    <row r="2775"/>
-    <row r="2776"/>
-    <row r="2777"/>
-    <row r="2778"/>
-    <row r="2779"/>
-    <row r="2780"/>
-    <row r="2781"/>
-    <row r="2782"/>
-    <row r="2783"/>
-    <row r="2784"/>
-    <row r="2785"/>
-    <row r="2786"/>
-    <row r="2787"/>
-    <row r="2788"/>
-    <row r="2789"/>
-    <row r="2790"/>
-    <row r="2791"/>
-    <row r="2792"/>
-    <row r="2793"/>
-    <row r="2794"/>
-    <row r="2795"/>
-    <row r="2796"/>
-    <row r="2797"/>
-    <row r="2798"/>
-    <row r="2799"/>
-    <row r="2800"/>
-    <row r="2801"/>
-    <row r="2802"/>
-    <row r="2803"/>
-    <row r="2804"/>
-    <row r="2805"/>
-    <row r="2806"/>
-    <row r="2807"/>
-    <row r="2808"/>
-    <row r="2809"/>
-    <row r="2810"/>
-    <row r="2811"/>
-    <row r="2812"/>
-    <row r="2813"/>
-    <row r="2814"/>
-    <row r="2815"/>
-    <row r="2816"/>
-    <row r="2817"/>
-    <row r="2818"/>
-    <row r="2819"/>
-    <row r="2820"/>
-    <row r="2821"/>
-    <row r="2822"/>
-    <row r="2823"/>
-    <row r="2824"/>
-    <row r="2825"/>
-    <row r="2826"/>
-    <row r="2827"/>
-    <row r="2828"/>
-    <row r="2829"/>
-    <row r="2830"/>
-    <row r="2831"/>
-    <row r="2832"/>
-    <row r="2833"/>
-    <row r="2834"/>
-    <row r="2835"/>
-    <row r="2836"/>
-    <row r="2837"/>
-    <row r="2838"/>
-    <row r="2839"/>
-    <row r="2840"/>
-    <row r="2841"/>
-    <row r="2842"/>
-    <row r="2843"/>
-    <row r="2844"/>
-    <row r="2845"/>
-    <row r="2846"/>
-    <row r="2847"/>
-    <row r="2848"/>
-    <row r="2849"/>
-    <row r="2850"/>
-    <row r="2851"/>
-    <row r="2852"/>
-    <row r="2853"/>
-    <row r="2854"/>
-    <row r="2855"/>
-    <row r="2856"/>
-    <row r="2857"/>
-    <row r="2858"/>
-    <row r="2859"/>
-    <row r="2860"/>
-    <row r="2861"/>
-    <row r="2862"/>
-    <row r="2863"/>
-    <row r="2864"/>
-    <row r="2865"/>
-    <row r="2866"/>
-    <row r="2867"/>
-    <row r="2868"/>
-    <row r="2869"/>
-    <row r="2870"/>
-    <row r="2871"/>
-    <row r="2872"/>
-    <row r="2873"/>
-    <row r="2874"/>
-    <row r="2875"/>
-    <row r="2876"/>
-    <row r="2877"/>
-    <row r="2878"/>
-    <row r="2879"/>
-    <row r="2880"/>
-    <row r="2881"/>
-    <row r="2882"/>
-    <row r="2883"/>
-    <row r="2884"/>
-    <row r="2885"/>
-    <row r="2886"/>
-    <row r="2887"/>
-    <row r="2888"/>
-    <row r="2889"/>
-    <row r="2890"/>
-    <row r="2891"/>
-    <row r="2892"/>
-    <row r="2893"/>
-    <row r="2894"/>
-    <row r="2895"/>
-    <row r="2896"/>
-    <row r="2897"/>
-    <row r="2898"/>
-    <row r="2899"/>
-    <row r="2900"/>
-    <row r="2901"/>
-    <row r="2902"/>
-    <row r="2903"/>
-    <row r="2904"/>
-    <row r="2905"/>
-    <row r="2906"/>
-    <row r="2907"/>
-    <row r="2908"/>
-    <row r="2909"/>
-    <row r="2910"/>
-    <row r="2911"/>
-    <row r="2912"/>
-    <row r="2913"/>
-    <row r="2914"/>
-    <row r="2915"/>
-    <row r="2916"/>
-    <row r="2917"/>
-    <row r="2918"/>
-    <row r="2919"/>
-    <row r="2920"/>
-    <row r="2921"/>
-    <row r="2922"/>
-    <row r="2923"/>
-    <row r="2924"/>
-    <row r="2925"/>
-    <row r="2926"/>
-    <row r="2927"/>
-    <row r="2928"/>
-    <row r="2929"/>
-    <row r="2930"/>
-    <row r="2931"/>
-    <row r="2932"/>
-    <row r="2933"/>
-    <row r="2934"/>
-    <row r="2935"/>
-    <row r="2936"/>
-    <row r="2937"/>
-    <row r="2938"/>
-    <row r="2939"/>
-    <row r="2940"/>
-    <row r="2941"/>
-    <row r="2942"/>
-    <row r="2943"/>
-    <row r="2944"/>
-    <row r="2945"/>
-    <row r="2946"/>
-    <row r="2947"/>
-    <row r="2948"/>
-    <row r="2949"/>
-    <row r="2950"/>
-    <row r="2951"/>
-    <row r="2952"/>
-    <row r="2953"/>
-    <row r="2954"/>
-    <row r="2955"/>
-    <row r="2956"/>
-    <row r="2957"/>
-    <row r="2958"/>
-    <row r="2959"/>
-    <row r="2960"/>
-    <row r="2961"/>
-    <row r="2962"/>
-    <row r="2963"/>
-    <row r="2964"/>
-    <row r="2965"/>
-    <row r="2966"/>
-    <row r="2967"/>
-    <row r="2968"/>
-    <row r="2969"/>
-    <row r="2970"/>
-    <row r="2971"/>
-    <row r="2972"/>
-    <row r="2973"/>
-    <row r="2974"/>
-    <row r="2975"/>
-    <row r="2976"/>
-    <row r="2977"/>
-    <row r="2978"/>
-    <row r="2979"/>
-    <row r="2980"/>
-    <row r="2981"/>
-    <row r="2982"/>
-    <row r="2983"/>
-    <row r="2984"/>
-    <row r="2985"/>
-    <row r="2986"/>
-    <row r="2987"/>
-    <row r="2988"/>
-    <row r="2989"/>
-    <row r="2990"/>
-    <row r="2991"/>
-    <row r="2992"/>
-    <row r="2993"/>
-    <row r="2994"/>
-    <row r="2995"/>
-    <row r="2996"/>
-    <row r="2997"/>
-    <row r="2998"/>
-    <row r="2999"/>
-    <row r="3000"/>
-    <row r="3001"/>
-    <row r="3002"/>
-    <row r="3003"/>
-    <row r="3004">
-      <c r="GL3004" s="7" t="inlineStr">
-        <is>
-          <t>Ingredients Table. List ingredients here with their respective weigher number and relative ordering (ordering is individual to each weigher, leave both blank if they are manually added).</t>
-        </is>
-      </c>
-      <c r="GM3004" s="8" t="n"/>
-      <c r="GN3004" s="8" t="n"/>
-      <c r="GP3004" s="7" t="inlineStr">
-        <is>
-          <t>Ration Table. List rations here with values for each ingredient in correct column, add ingredients to match ingredients table to end of table.</t>
-        </is>
-      </c>
-      <c r="GQ3004" s="8" t="n"/>
-      <c r="GR3004" s="8" t="n"/>
-      <c r="GS3004" s="8" t="n"/>
-      <c r="GT3004" s="8" t="n"/>
-      <c r="GU3004" s="8" t="n"/>
-      <c r="GV3004" s="8" t="n"/>
-      <c r="GW3004" s="8" t="n"/>
-      <c r="GX3004" s="8" t="n"/>
-      <c r="GY3004" s="7" t="n"/>
-      <c r="GZ3004" s="8" t="n"/>
-      <c r="HC3004" s="7" t="inlineStr">
-        <is>
-          <t>House Table. List the house names here</t>
-        </is>
-      </c>
-      <c r="HE3004" s="7" t="inlineStr">
-        <is>
-          <t>Weigher Table, gives weigher numbers and the value they increment by each time</t>
-        </is>
-      </c>
-      <c r="HF3004" s="7" t="n"/>
-    </row>
-    <row r="3005">
-      <c r="GL3005" s="4" t="inlineStr">
-        <is>
-          <t>Ingredient</t>
-        </is>
-      </c>
-      <c r="GM3005" s="5" t="inlineStr">
-        <is>
-          <t>Weigher</t>
-        </is>
-      </c>
-      <c r="GN3005" s="6" t="inlineStr">
-        <is>
-          <t>Ordering</t>
-        </is>
-      </c>
-      <c r="GP3005" s="4" t="inlineStr">
-        <is>
-          <t>Ration</t>
-        </is>
-      </c>
-      <c r="GQ3005" s="5" t="inlineStr">
-        <is>
-          <t>Barley</t>
-        </is>
-      </c>
-      <c r="GR3005" s="5" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
-      <c r="GS3005" s="5" t="inlineStr">
-        <is>
-          <t>Soya</t>
-        </is>
-      </c>
-      <c r="GT3005" s="5" t="inlineStr">
-        <is>
-          <t>Limestone</t>
-        </is>
-      </c>
-      <c r="GU3005" s="5" t="inlineStr">
-        <is>
-          <t>Soya Oil</t>
-        </is>
-      </c>
-      <c r="GV3005" s="5" t="inlineStr">
-        <is>
-          <t>Methionine</t>
-        </is>
-      </c>
-      <c r="GW3005" s="5" t="inlineStr">
-        <is>
-          <t>Arbocell</t>
-        </is>
-      </c>
-      <c r="GX3005" s="6" t="inlineStr">
-        <is>
-          <t>Premix</t>
-        </is>
-      </c>
-      <c r="GY3005" s="7" t="inlineStr">
-        <is>
-          <t>Extra Ingred</t>
-        </is>
-      </c>
-      <c r="GZ3005" s="8" t="inlineStr">
-        <is>
-          <t>Extra Ingred 2</t>
-        </is>
-      </c>
-      <c r="HC3005" s="9" t="inlineStr">
-        <is>
-          <t>Houses</t>
-        </is>
-      </c>
-      <c r="HE3005" s="7" t="inlineStr">
-        <is>
-          <t>Weighers</t>
-        </is>
-      </c>
-      <c r="HF3005" s="7" t="inlineStr">
-        <is>
-          <t>Increment</t>
-        </is>
-      </c>
-    </row>
-    <row r="3006">
-      <c r="GL3006" s="7" t="inlineStr">
-        <is>
-          <t>Barley</t>
-        </is>
-      </c>
-      <c r="GM3006" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="GN3006" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="GP3006" s="7" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="GQ3006" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GR3006" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GS3006" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GT3006" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GU3006" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GV3006" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GW3006" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GX3006" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GY3006" s="7" t="n">
-        <v>420</v>
-      </c>
-      <c r="GZ3006" s="8" t="n"/>
-      <c r="HC3006" s="7" t="inlineStr">
-        <is>
-          <t>House 1</t>
-        </is>
-      </c>
-      <c r="HE3006" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="HF3006" s="7" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3007">
-      <c r="GL3007" s="8" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
-      <c r="GM3007" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="GN3007" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="GP3007" s="7" t="inlineStr">
-        <is>
-          <t>Peak Lay</t>
-        </is>
-      </c>
-      <c r="GQ3007" s="7" t="n">
-        <v>300</v>
-      </c>
-      <c r="GR3007" s="7" t="n">
-        <v>560</v>
-      </c>
-      <c r="GS3007" s="7" t="n">
-        <v>210</v>
-      </c>
-      <c r="GT3007" s="7" t="n">
-        <v>58</v>
-      </c>
-      <c r="GU3007" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="GV3007" s="7" t="n">
-        <v>20</v>
-      </c>
-      <c r="GW3007" s="7" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="GX3007" s="7" t="n">
-        <v>40</v>
-      </c>
-      <c r="GY3007" s="7" t="n">
-        <v>32</v>
-      </c>
-      <c r="GZ3007" s="8" t="n">
-        <v>32</v>
-      </c>
-      <c r="HC3007" s="7" t="inlineStr">
-        <is>
-          <t>House 2</t>
-        </is>
-      </c>
-      <c r="HE3007" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="HF3007" s="7" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3008">
-      <c r="GL3008" s="7" t="inlineStr">
-        <is>
-          <t>Soya</t>
-        </is>
-      </c>
-      <c r="GM3008" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="GN3008" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="GP3008" s="7" t="inlineStr">
-        <is>
-          <t>Mid Lay</t>
-        </is>
-      </c>
-      <c r="GQ3008" s="7" t="n">
-        <v>50</v>
-      </c>
-      <c r="GR3008" s="7" t="n">
-        <v>20</v>
-      </c>
-      <c r="GS3008" s="7" t="n">
-        <v>62</v>
-      </c>
-      <c r="GT3008" s="7" t="n">
-        <v>51</v>
-      </c>
-      <c r="GU3008" s="7" t="n">
-        <v>866</v>
-      </c>
-      <c r="GV3008" s="7" t="n">
-        <v>23</v>
-      </c>
-      <c r="GW3008" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="GX3008" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="GY3008" s="7" t="n">
-        <v>32</v>
-      </c>
-      <c r="GZ3008" s="8" t="n">
-        <v>32</v>
-      </c>
-      <c r="HC3008" s="7" t="inlineStr">
-        <is>
-          <t>House 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="3009">
-      <c r="GL3009" s="7" t="inlineStr">
-        <is>
-          <t>Limestone</t>
-        </is>
-      </c>
-      <c r="GM3009" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="GN3009" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="GP3009" s="7" t="inlineStr">
-        <is>
-          <t>Other Ration 1</t>
-        </is>
-      </c>
-      <c r="GQ3009" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GR3009" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GS3009" s="7" t="n"/>
-      <c r="GT3009" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GU3009" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GV3009" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GW3009" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GX3009" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GY3009" s="7" t="n">
-        <v>32</v>
-      </c>
-      <c r="GZ3009" s="8" t="n">
-        <v>32</v>
-      </c>
-      <c r="HC3009" s="7" t="inlineStr">
-        <is>
-          <t>Manor Wood</t>
-        </is>
-      </c>
-    </row>
-    <row r="3010">
-      <c r="GL3010" s="10" t="inlineStr">
-        <is>
-          <t>Extra Ingred</t>
-        </is>
-      </c>
-      <c r="GM3010" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="GN3010" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="GP3010" s="7" t="inlineStr">
-        <is>
-          <t>Other Ration 2</t>
-        </is>
-      </c>
-      <c r="GQ3010" s="7" t="n">
-        <v>300</v>
-      </c>
-      <c r="GR3010" s="7" t="n">
-        <v>560</v>
-      </c>
-      <c r="GS3010" s="7" t="n">
-        <v>210</v>
-      </c>
-      <c r="GT3010" s="7" t="n">
-        <v>58</v>
-      </c>
-      <c r="GU3010" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="GV3010" s="7" t="n">
-        <v>20</v>
-      </c>
-      <c r="GW3010" s="7" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="GX3010" s="7" t="n">
-        <v>40</v>
-      </c>
-      <c r="GY3010" s="7" t="n">
-        <v>32</v>
-      </c>
-      <c r="GZ3010" s="8" t="n">
-        <v>32</v>
-      </c>
-      <c r="HC3010" s="7" t="inlineStr">
-        <is>
-          <t>Wawne Hill</t>
-        </is>
-      </c>
-    </row>
-    <row r="3011">
-      <c r="GL3011" s="10" t="inlineStr">
-        <is>
-          <t>Extra Ingred 2</t>
-        </is>
-      </c>
-      <c r="GM3011" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="GN3011" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="GP3011" s="7" t="inlineStr">
-        <is>
-          <t>Other Ration 3</t>
-        </is>
-      </c>
-      <c r="GQ3011" s="7" t="n">
-        <v>50</v>
-      </c>
-      <c r="GR3011" s="7" t="n">
-        <v>20</v>
-      </c>
-      <c r="GS3011" s="7" t="n">
-        <v>62</v>
-      </c>
-      <c r="GT3011" s="7" t="n">
-        <v>51</v>
-      </c>
-      <c r="GU3011" s="7" t="n">
-        <v>866</v>
-      </c>
-      <c r="GV3011" s="7" t="n">
-        <v>23</v>
-      </c>
-      <c r="GW3011" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="GX3011" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="GY3011" s="7" t="n">
-        <v>32</v>
-      </c>
-      <c r="GZ3011" s="7" t="n"/>
-      <c r="HC3011" s="7" t="inlineStr">
-        <is>
-          <t>House 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="3012">
-      <c r="GL3012" s="7" t="inlineStr">
-        <is>
-          <t>Soya Oil</t>
-        </is>
-      </c>
-      <c r="GM3012" s="7" t="n"/>
-      <c r="GN3012" s="7" t="n"/>
-      <c r="GP3012" s="7" t="inlineStr">
-        <is>
-          <t>Other Ration 4</t>
-        </is>
-      </c>
-      <c r="GQ3012" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GR3012" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GS3012" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GT3012" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GU3012" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GV3012" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GW3012" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GX3012" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GY3012" s="7" t="n">
-        <v>32</v>
-      </c>
-      <c r="GZ3012" s="7" t="n"/>
-      <c r="HC3012" s="7" t="inlineStr">
-        <is>
-          <t>House 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="3013">
-      <c r="GL3013" s="7" t="inlineStr">
-        <is>
-          <t>Methionine</t>
-        </is>
-      </c>
-      <c r="GM3013" s="7" t="n"/>
-      <c r="GN3013" s="7" t="n"/>
-      <c r="GP3013" s="7" t="inlineStr">
-        <is>
-          <t>Other Ration 5</t>
-        </is>
-      </c>
-      <c r="GQ3013" s="7" t="n">
-        <v>300</v>
-      </c>
-      <c r="GR3013" s="7" t="n">
-        <v>560</v>
-      </c>
-      <c r="GS3013" s="7" t="n">
-        <v>210</v>
-      </c>
-      <c r="GT3013" s="7" t="n">
-        <v>58</v>
-      </c>
-      <c r="GU3013" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="GV3013" s="7" t="n">
-        <v>20</v>
-      </c>
-      <c r="GW3013" s="7" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="GX3013" s="7" t="n">
-        <v>40</v>
-      </c>
-      <c r="GY3013" s="7" t="n">
-        <v>32</v>
-      </c>
-      <c r="GZ3013" s="7" t="n"/>
-      <c r="HC3013" s="7" t="inlineStr">
-        <is>
-          <t>House 6</t>
-        </is>
-      </c>
-    </row>
-    <row r="3014">
-      <c r="GL3014" s="7" t="inlineStr">
-        <is>
-          <t>Arbocell</t>
-        </is>
-      </c>
-      <c r="GM3014" s="7" t="n"/>
-      <c r="GN3014" s="7" t="n"/>
-      <c r="GP3014" s="7" t="inlineStr">
-        <is>
-          <t>Other Ration 6</t>
-        </is>
-      </c>
-      <c r="GQ3014" s="7" t="n">
-        <v>50</v>
-      </c>
-      <c r="GR3014" s="7" t="n">
-        <v>20</v>
-      </c>
-      <c r="GS3014" s="7" t="n">
-        <v>62</v>
-      </c>
-      <c r="GT3014" s="7" t="n">
-        <v>51</v>
-      </c>
-      <c r="GU3014" s="7" t="n">
-        <v>866</v>
-      </c>
-      <c r="GV3014" s="7" t="n">
-        <v>23</v>
-      </c>
-      <c r="GW3014" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="GX3014" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="GY3014" s="7" t="n">
-        <v>32</v>
-      </c>
-      <c r="GZ3014" s="7" t="n"/>
-      <c r="HC3014" s="7" t="inlineStr">
-        <is>
-          <t>House 7</t>
-        </is>
-      </c>
-    </row>
-    <row r="3015">
-      <c r="GL3015" s="7" t="inlineStr">
-        <is>
-          <t>Premix</t>
-        </is>
-      </c>
-      <c r="GM3015" s="7" t="n"/>
-      <c r="GN3015" s="7" t="n"/>
-      <c r="GP3015" s="7" t="inlineStr">
-        <is>
-          <t>Other Ration 7</t>
-        </is>
-      </c>
-      <c r="GQ3015" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GR3015" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GS3015" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GT3015" s="7" t="n"/>
-      <c r="GU3015" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GV3015" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GW3015" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GX3015" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="GY3015" s="7" t="n">
-        <v>600</v>
-      </c>
-      <c r="GZ3015" s="7" t="n"/>
-      <c r="HC3015" s="7" t="inlineStr">
-        <is>
-          <t>House 8</t>
-        </is>
-      </c>
-    </row>
-    <row r="3016">
-      <c r="GP3016" s="7" t="inlineStr">
-        <is>
-          <t>Other Ration 8</t>
-        </is>
-      </c>
-      <c r="GQ3016" s="7" t="n">
-        <v>300</v>
-      </c>
-      <c r="GR3016" s="7" t="n">
-        <v>560</v>
-      </c>
-      <c r="GS3016" s="7" t="n">
-        <v>210</v>
-      </c>
-      <c r="GT3016" s="7" t="n">
-        <v>58</v>
-      </c>
-      <c r="GU3016" s="7" t="n">
-        <v>100</v>
-      </c>
-      <c r="GV3016" s="7" t="n">
-        <v>20</v>
-      </c>
-      <c r="GW3016" s="7" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="GX3016" s="7" t="n">
-        <v>40</v>
-      </c>
-      <c r="GY3016" s="7" t="n"/>
-      <c r="GZ3016" s="7" t="n"/>
-      <c r="HC3016" s="7" t="inlineStr">
-        <is>
-          <t>House 9</t>
-        </is>
-      </c>
-    </row>
-    <row r="3017">
-      <c r="GP3017" s="7" t="inlineStr">
-        <is>
-          <t>Other Ration 9</t>
-        </is>
-      </c>
-      <c r="GQ3017" s="7" t="n">
-        <v>50</v>
-      </c>
-      <c r="GR3017" s="7" t="n">
-        <v>20</v>
-      </c>
-      <c r="GS3017" s="7" t="n">
-        <v>62</v>
-      </c>
-      <c r="GT3017" s="7" t="n">
-        <v>51</v>
-      </c>
-      <c r="GU3017" s="7" t="n">
-        <v>866</v>
-      </c>
-      <c r="GV3017" s="7" t="n">
-        <v>23</v>
-      </c>
-      <c r="GW3017" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="GX3017" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="GY3017" s="7" t="n"/>
-      <c r="GZ3017" s="7" t="n"/>
-      <c r="HC3017" s="7" t="inlineStr">
-        <is>
-          <t>House 10</t>
-        </is>
-      </c>
-    </row>
-    <row r="3018">
-      <c r="HC3018" s="7" t="inlineStr">
-        <is>
-          <t>House 11</t>
-        </is>
-      </c>
-    </row>
-    <row r="3019">
-      <c r="HC3019" s="7" t="inlineStr">
-        <is>
-          <t>House 12</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>